<commit_message>
Se agrega honorarios al generador!
</commit_message>
<xml_diff>
--- a/catalogo.xlsx
+++ b/catalogo.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="118">
   <si>
     <t>NOMBRE DE LA COLUMNA</t>
   </si>
@@ -373,6 +373,12 @@
   </si>
   <si>
     <t>ADEUDO A FINANZAS</t>
+  </si>
+  <si>
+    <t>GRATIFICACION RETROACTIVA</t>
+  </si>
+  <si>
+    <t>RETRO_GRAT</t>
   </si>
 </sst>
 </file>
@@ -444,15 +450,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -733,10 +739,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G45"/>
+  <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1223,7 +1229,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -1232,7 +1238,7 @@
         <v>76</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>113</v>
@@ -1243,19 +1249,19 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B25">
         <v>1</v>
       </c>
-      <c r="C25">
-        <v>1204</v>
-      </c>
-      <c r="D25" t="s">
-        <v>111</v>
+      <c r="C25" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>112</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>78</v>
+        <v>113</v>
       </c>
       <c r="F25">
         <v>0</v>
@@ -1263,39 +1269,39 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>75</v>
+        <v>110</v>
       </c>
       <c r="B26">
-        <v>2</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>75</v>
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>1204</v>
+      </c>
+      <c r="D26" t="s">
+        <v>111</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F26">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>16</v>
+        <v>75</v>
       </c>
       <c r="B27">
         <v>2</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="D27" t="s">
-        <v>17</v>
+        <v>76</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>75</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F27">
         <v>1</v>
@@ -1303,19 +1309,19 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B28">
         <v>2</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>79</v>
+        <v>92</v>
       </c>
       <c r="D28" t="s">
-        <v>103</v>
-      </c>
-      <c r="E28" s="6" t="s">
-        <v>87</v>
+        <v>17</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>80</v>
       </c>
       <c r="F28">
         <v>1</v>
@@ -1323,19 +1329,19 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B29">
         <v>2</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D29" t="s">
-        <v>104</v>
-      </c>
-      <c r="E29" s="5" t="s">
-        <v>76</v>
+        <v>103</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>87</v>
       </c>
       <c r="F29">
         <v>1</v>
@@ -1343,19 +1349,19 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B30">
         <v>2</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="D30" t="s">
-        <v>21</v>
+        <v>104</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="F30">
         <v>1</v>
@@ -1363,19 +1369,19 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B31">
         <v>2</v>
       </c>
       <c r="C31" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D31" t="s">
+        <v>21</v>
+      </c>
+      <c r="E31" s="5" t="s">
         <v>87</v>
-      </c>
-      <c r="D31" t="s">
-        <v>23</v>
-      </c>
-      <c r="E31" s="5" t="s">
-        <v>83</v>
       </c>
       <c r="F31">
         <v>1</v>
@@ -1383,19 +1389,19 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B32">
         <v>2</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="D32" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F32">
         <v>1</v>
@@ -1403,19 +1409,19 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B33">
         <v>2</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D33" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F33">
         <v>1</v>
@@ -1423,7 +1429,7 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B34">
         <v>2</v>
@@ -1443,16 +1449,16 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B35">
         <v>2</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D35" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E35" s="5" t="s">
         <v>83</v>
@@ -1463,16 +1469,16 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B36">
         <v>2</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D36" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E36" s="5" t="s">
         <v>83</v>
@@ -1483,16 +1489,16 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B37">
         <v>2</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D37" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E37" s="5" t="s">
         <v>83</v>
@@ -1503,16 +1509,16 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B38">
         <v>2</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D38" t="s">
-        <v>86</v>
+        <v>33</v>
       </c>
       <c r="E38" s="5" t="s">
         <v>83</v>
@@ -1523,7 +1529,7 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B39">
         <v>2</v>
@@ -1531,8 +1537,8 @@
       <c r="C39" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="D39" s="3" t="s">
-        <v>41</v>
+      <c r="D39" t="s">
+        <v>86</v>
       </c>
       <c r="E39" s="5" t="s">
         <v>83</v>
@@ -1540,22 +1546,19 @@
       <c r="F39">
         <v>1</v>
       </c>
-      <c r="G39" s="9" t="s">
-        <v>68</v>
-      </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B40">
         <v>2</v>
       </c>
-      <c r="C40" s="8" t="s">
-        <v>100</v>
+      <c r="C40" s="5" t="s">
+        <v>99</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E40" s="5" t="s">
         <v>83</v>
@@ -1563,121 +1566,144 @@
       <c r="F40">
         <v>1</v>
       </c>
-      <c r="G40" s="9"/>
+      <c r="G40" s="12" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B41">
         <v>2</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F41">
         <v>1</v>
       </c>
-      <c r="G41" s="10" t="s">
-        <v>44</v>
-      </c>
+      <c r="G41" s="12"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B42">
         <v>2</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="F42" s="4">
-        <v>1</v>
-      </c>
-      <c r="G42" s="10"/>
+        <v>81</v>
+      </c>
+      <c r="F42">
+        <v>1</v>
+      </c>
+      <c r="G42" s="13" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>73</v>
+        <v>45</v>
       </c>
       <c r="B43">
         <v>2</v>
       </c>
-      <c r="C43" s="5" t="s">
-        <v>102</v>
+      <c r="C43" s="8" t="s">
+        <v>91</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="E43" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="F43">
-        <v>1</v>
-      </c>
-      <c r="G43" s="3" t="s">
+      <c r="F43" s="4">
+        <v>1</v>
+      </c>
+      <c r="G43" s="13"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>73</v>
+      </c>
+      <c r="B44">
+        <v>2</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="F44">
+        <v>1</v>
+      </c>
+      <c r="G44" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="44" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="13" t="s">
+    <row r="45" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="B44" s="1">
-        <v>2</v>
-      </c>
-      <c r="C44" s="11" t="s">
+      <c r="B45" s="1">
+        <v>2</v>
+      </c>
+      <c r="C45" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="D44" s="1" t="s">
+      <c r="D45" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="E44" s="11" t="s">
+      <c r="E45" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="F44" s="1">
-        <v>1</v>
-      </c>
-      <c r="G44" s="12"/>
-    </row>
-    <row r="45" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
+      <c r="F45" s="1">
+        <v>1</v>
+      </c>
+      <c r="G45" s="10"/>
+    </row>
+    <row r="46" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B45" s="1">
-        <v>2</v>
-      </c>
-      <c r="C45" s="11" t="s">
+      <c r="B46" s="1">
+        <v>2</v>
+      </c>
+      <c r="C46" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="D45" s="1" t="s">
+      <c r="D46" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="E45" s="11" t="s">
+      <c r="E46" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="F45" s="1">
-        <v>1</v>
-      </c>
-      <c r="G45" s="12"/>
+      <c r="F46" s="1">
+        <v>1</v>
+      </c>
+      <c r="G46" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="G39:G40"/>
-    <mergeCell ref="G41:G42"/>
+    <mergeCell ref="G40:G41"/>
+    <mergeCell ref="G42:G43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Generando plantillas para compensaciones
</commit_message>
<xml_diff>
--- a/catalogo.xlsx
+++ b/catalogo.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="120">
   <si>
     <t>NOMBRE DE LA COLUMNA</t>
   </si>
@@ -379,6 +379,12 @@
   </si>
   <si>
     <t>RETRO_GRAT</t>
+  </si>
+  <si>
+    <t>COMPENSACION_ADMINISTRATIVA_RETRO</t>
+  </si>
+  <si>
+    <t>COMPENSACION ADMINISTRATIVA RETROACTIVA</t>
   </si>
 </sst>
 </file>
@@ -739,10 +745,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G46"/>
+  <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -977,7 +983,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>106</v>
+        <v>118</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -986,7 +992,7 @@
         <v>1102</v>
       </c>
       <c r="D12" t="s">
-        <v>107</v>
+        <v>119</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>78</v>
@@ -997,16 +1003,16 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>39</v>
+        <v>106</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
       <c r="C13">
-        <v>1204</v>
+        <v>1102</v>
       </c>
       <c r="D13" t="s">
-        <v>85</v>
+        <v>107</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>78</v>
@@ -1017,16 +1023,16 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>70</v>
+        <v>39</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
-      <c r="C14" s="5" t="s">
-        <v>88</v>
+      <c r="C14">
+        <v>1204</v>
       </c>
       <c r="D14" t="s">
-        <v>37</v>
+        <v>85</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>78</v>
@@ -1037,16 +1043,16 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
-      <c r="C15">
-        <v>1326</v>
+      <c r="C15" s="5" t="s">
+        <v>88</v>
       </c>
       <c r="D15" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>78</v>
@@ -1057,19 +1063,19 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
       <c r="C16">
-        <v>1601</v>
+        <v>1326</v>
       </c>
       <c r="D16" t="s">
-        <v>61</v>
+        <v>39</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F16">
         <v>0</v>
@@ -1077,19 +1083,19 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
       <c r="C17">
-        <v>1099</v>
+        <v>1601</v>
       </c>
       <c r="D17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F17">
         <v>0</v>
@@ -1097,16 +1103,16 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
-      <c r="C18" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>53</v>
+      <c r="C18">
+        <v>1099</v>
+      </c>
+      <c r="D18" t="s">
+        <v>62</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>78</v>
@@ -1117,39 +1123,36 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B19">
         <v>1</v>
       </c>
-      <c r="C19" s="2">
-        <v>1317</v>
+      <c r="C19" s="7" t="s">
+        <v>89</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>78</v>
       </c>
       <c r="F19">
         <v>0</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
-      <c r="C20" s="7" t="s">
-        <v>90</v>
+      <c r="C20" s="2">
+        <v>1317</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>78</v>
@@ -1158,21 +1161,21 @@
         <v>0</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B21">
         <v>1</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>78</v>
@@ -1181,21 +1184,21 @@
         <v>0</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="B22">
         <v>1</v>
       </c>
-      <c r="C22" s="2">
-        <v>1337</v>
+      <c r="C22" s="7" t="s">
+        <v>91</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>78</v>
@@ -1204,44 +1207,47 @@
         <v>0</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B23">
         <v>1</v>
       </c>
       <c r="C23" s="2">
-        <v>1710</v>
+        <v>1337</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>78</v>
       </c>
       <c r="F23">
         <v>0</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>117</v>
+        <v>49</v>
       </c>
       <c r="B24">
         <v>1</v>
       </c>
-      <c r="C24" s="7" t="s">
-        <v>76</v>
+      <c r="C24" s="2">
+        <v>1710</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>116</v>
+        <v>50</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>113</v>
+        <v>78</v>
       </c>
       <c r="F24">
         <v>0</v>
@@ -1249,7 +1255,7 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -1258,7 +1264,7 @@
         <v>76</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="E25" s="5" t="s">
         <v>113</v>
@@ -1269,19 +1275,19 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B26">
         <v>1</v>
       </c>
-      <c r="C26">
-        <v>1204</v>
-      </c>
-      <c r="D26" t="s">
-        <v>111</v>
+      <c r="C26" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>112</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>78</v>
+        <v>113</v>
       </c>
       <c r="F26">
         <v>0</v>
@@ -1289,39 +1295,39 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>75</v>
+        <v>110</v>
       </c>
       <c r="B27">
-        <v>2</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>75</v>
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <v>1204</v>
+      </c>
+      <c r="D27" t="s">
+        <v>111</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F27">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>16</v>
+        <v>75</v>
       </c>
       <c r="B28">
         <v>2</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="D28" t="s">
-        <v>17</v>
+        <v>76</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>75</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F28">
         <v>1</v>
@@ -1329,19 +1335,19 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B29">
         <v>2</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>79</v>
+        <v>92</v>
       </c>
       <c r="D29" t="s">
-        <v>103</v>
-      </c>
-      <c r="E29" s="6" t="s">
-        <v>87</v>
+        <v>17</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>80</v>
       </c>
       <c r="F29">
         <v>1</v>
@@ -1349,19 +1355,19 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B30">
         <v>2</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D30" t="s">
-        <v>104</v>
-      </c>
-      <c r="E30" s="5" t="s">
-        <v>76</v>
+        <v>103</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>87</v>
       </c>
       <c r="F30">
         <v>1</v>
@@ -1369,19 +1375,19 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B31">
         <v>2</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="D31" t="s">
-        <v>21</v>
+        <v>104</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="F31">
         <v>1</v>
@@ -1389,19 +1395,19 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B32">
         <v>2</v>
       </c>
       <c r="C32" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D32" t="s">
+        <v>21</v>
+      </c>
+      <c r="E32" s="5" t="s">
         <v>87</v>
-      </c>
-      <c r="D32" t="s">
-        <v>23</v>
-      </c>
-      <c r="E32" s="5" t="s">
-        <v>83</v>
       </c>
       <c r="F32">
         <v>1</v>
@@ -1409,19 +1415,19 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B33">
         <v>2</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="D33" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F33">
         <v>1</v>
@@ -1429,19 +1435,19 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B34">
         <v>2</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D34" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F34">
         <v>1</v>
@@ -1449,7 +1455,7 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B35">
         <v>2</v>
@@ -1469,16 +1475,16 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B36">
         <v>2</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D36" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E36" s="5" t="s">
         <v>83</v>
@@ -1489,16 +1495,16 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B37">
         <v>2</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D37" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E37" s="5" t="s">
         <v>83</v>
@@ -1509,16 +1515,16 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B38">
         <v>2</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D38" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E38" s="5" t="s">
         <v>83</v>
@@ -1529,16 +1535,16 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B39">
         <v>2</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D39" t="s">
-        <v>86</v>
+        <v>33</v>
       </c>
       <c r="E39" s="5" t="s">
         <v>83</v>
@@ -1549,7 +1555,7 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B40">
         <v>2</v>
@@ -1557,8 +1563,8 @@
       <c r="C40" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="D40" s="3" t="s">
-        <v>41</v>
+      <c r="D40" t="s">
+        <v>86</v>
       </c>
       <c r="E40" s="5" t="s">
         <v>83</v>
@@ -1566,22 +1572,19 @@
       <c r="F40">
         <v>1</v>
       </c>
-      <c r="G40" s="12" t="s">
-        <v>68</v>
-      </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B41">
         <v>2</v>
       </c>
-      <c r="C41" s="8" t="s">
-        <v>100</v>
+      <c r="C41" s="5" t="s">
+        <v>99</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E41" s="5" t="s">
         <v>83</v>
@@ -1589,99 +1592,101 @@
       <c r="F41">
         <v>1</v>
       </c>
-      <c r="G41" s="12"/>
+      <c r="G41" s="12" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B42">
         <v>2</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F42">
         <v>1</v>
       </c>
-      <c r="G42" s="13" t="s">
-        <v>44</v>
-      </c>
+      <c r="G42" s="12"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B43">
         <v>2</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="F43" s="4">
-        <v>1</v>
-      </c>
-      <c r="G43" s="13"/>
+        <v>81</v>
+      </c>
+      <c r="F43">
+        <v>1</v>
+      </c>
+      <c r="G43" s="13" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>73</v>
+        <v>45</v>
       </c>
       <c r="B44">
         <v>2</v>
       </c>
-      <c r="C44" s="5" t="s">
-        <v>102</v>
+      <c r="C44" s="8" t="s">
+        <v>91</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="E44" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="F44">
-        <v>1</v>
-      </c>
-      <c r="G44" s="3" t="s">
+      <c r="F44" s="4">
+        <v>1</v>
+      </c>
+      <c r="G44" s="13"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>73</v>
+      </c>
+      <c r="B45">
+        <v>2</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="F45">
+        <v>1</v>
+      </c>
+      <c r="G45" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="45" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="11" t="s">
+    <row r="46" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="11" t="s">
         <v>68</v>
-      </c>
-      <c r="B45" s="1">
-        <v>2</v>
-      </c>
-      <c r="C45" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="E45" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="F45" s="1">
-        <v>1</v>
-      </c>
-      <c r="G45" s="10"/>
-    </row>
-    <row r="46" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
-        <v>114</v>
       </c>
       <c r="B46" s="1">
         <v>2</v>
@@ -1690,7 +1695,7 @@
         <v>99</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>115</v>
+        <v>86</v>
       </c>
       <c r="E46" s="9" t="s">
         <v>83</v>
@@ -1700,10 +1705,31 @@
       </c>
       <c r="G46" s="10"/>
     </row>
+    <row r="47" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B47" s="1">
+        <v>2</v>
+      </c>
+      <c r="C47" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E47" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="F47" s="1">
+        <v>1</v>
+      </c>
+      <c r="G47" s="10"/>
+    </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="G40:G41"/>
-    <mergeCell ref="G42:G43"/>
+    <mergeCell ref="G41:G42"/>
+    <mergeCell ref="G43:G44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>